<commit_message>
WhiteBox 1 og 2 Done
</commit_message>
<xml_diff>
--- a/Documentation, figures, etc/WhiteBoxTests.xlsx
+++ b/Documentation, figures, etc/WhiteBoxTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s204472_dtu_dk/Documents/DTU/02161_Software_Engineering_1/Project/Project/SoftwareEngineering02161/Documentation, figures, etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{A437F17A-5F34-4C3A-9B66-3EB13CFEAD13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4B0B07E3-510E-457D-BD24-D3A9B41BF2D0}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{A437F17A-5F34-4C3A-9B66-3EB13CFEAD13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{80ECDC6B-5B93-4E7A-ADE2-8284ECDBE90F}"/>
   <bookViews>
-    <workbookView xWindow="-47115" yWindow="8925" windowWidth="17880" windowHeight="15660" xr2:uid="{DF258800-DD81-4D43-B493-28BED55C5AE6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{DF258800-DD81-4D43-B493-28BED55C5AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -711,7 +711,7 @@
   <dimension ref="A4:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="H3" sqref="H3:S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>